<commit_message>
performance measurements for multibeggar plot_portfolio_complexity() [close #3]
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_x_large_portfolio_complexity_data.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_x_large_portfolio_complexity_data.xlsx
@@ -468,7 +468,7 @@
         <v>43075</v>
       </c>
       <c r="C3" t="n">
-        <v>1.002640412091776</v>
+        <v>1.007409754992392</v>
       </c>
     </row>
     <row r="4">
@@ -479,7 +479,7 @@
         <v>43080</v>
       </c>
       <c r="C4" t="n">
-        <v>1.007422572959666</v>
+        <v>1.023256515285222</v>
       </c>
     </row>
     <row r="5">
@@ -490,7 +490,7 @@
         <v>43081</v>
       </c>
       <c r="C5" t="n">
-        <v>1.008593553503398</v>
+        <v>1.032378615180878</v>
       </c>
     </row>
     <row r="6">
@@ -501,7 +501,7 @@
         <v>43082</v>
       </c>
       <c r="C6" t="n">
-        <v>1.00567469577919</v>
+        <v>1.035232034502614</v>
       </c>
     </row>
     <row r="7">
@@ -512,7 +512,7 @@
         <v>43083</v>
       </c>
       <c r="C7" t="n">
-        <v>1.005037152092608</v>
+        <v>1.035858061394269</v>
       </c>
     </row>
     <row r="8">
@@ -523,7 +523,7 @@
         <v>43084</v>
       </c>
       <c r="C8" t="n">
-        <v>1.008985090715276</v>
+        <v>1.033693393640186</v>
       </c>
     </row>
     <row r="9">
@@ -534,7 +534,7 @@
         <v>43087</v>
       </c>
       <c r="C9" t="n">
-        <v>1.011341594101418</v>
+        <v>1.023769447580116</v>
       </c>
     </row>
     <row r="10">
@@ -545,7 +545,7 @@
         <v>43097</v>
       </c>
       <c r="C10" t="n">
-        <v>1.021326642889422</v>
+        <v>1.036886819904187</v>
       </c>
     </row>
     <row r="11">
@@ -556,7 +556,7 @@
         <v>43098</v>
       </c>
       <c r="C11" t="n">
-        <v>1.030518955451949</v>
+        <v>1.043568036796435</v>
       </c>
     </row>
     <row r="12">
@@ -567,7 +567,7 @@
         <v>43105</v>
       </c>
       <c r="C12" t="n">
-        <v>1.030347646205691</v>
+        <v>1.042369352336359</v>
       </c>
     </row>
     <row r="13">
@@ -578,7 +578,7 @@
         <v>43108</v>
       </c>
       <c r="C13" t="n">
-        <v>1.030569953442986</v>
+        <v>1.040573689259489</v>
       </c>
     </row>
     <row r="14">
@@ -589,7 +589,7 @@
         <v>43110</v>
       </c>
       <c r="C14" t="n">
-        <v>1.030237805734421</v>
+        <v>1.039886656710098</v>
       </c>
     </row>
     <row r="15">
@@ -600,7 +600,7 @@
         <v>43118</v>
       </c>
       <c r="C15" t="n">
-        <v>1.041728768737324</v>
+        <v>1.059620001939866</v>
       </c>
     </row>
     <row r="16">
@@ -611,7 +611,7 @@
         <v>43123</v>
       </c>
       <c r="C16" t="n">
-        <v>1.036327405919272</v>
+        <v>1.05357300610626</v>
       </c>
     </row>
     <row r="17">
@@ -622,7 +622,7 @@
         <v>43124</v>
       </c>
       <c r="C17" t="n">
-        <v>1.038431874400673</v>
+        <v>1.061513169202268</v>
       </c>
     </row>
     <row r="18">
@@ -633,7 +633,7 @@
         <v>43125</v>
       </c>
       <c r="C18" t="n">
-        <v>1.039023044389526</v>
+        <v>1.059752046391173</v>
       </c>
     </row>
     <row r="19">
@@ -644,7 +644,7 @@
         <v>43129</v>
       </c>
       <c r="C19" t="n">
-        <v>1.039398676147721</v>
+        <v>1.059473960793328</v>
       </c>
     </row>
     <row r="20">
@@ -655,7 +655,7 @@
         <v>43130</v>
       </c>
       <c r="C20" t="n">
-        <v>1.040051159122622</v>
+        <v>1.058761149729646</v>
       </c>
     </row>
     <row r="21">
@@ -666,7 +666,7 @@
         <v>43131</v>
       </c>
       <c r="C21" t="n">
-        <v>1.043657383378798</v>
+        <v>1.064467995877085</v>
       </c>
     </row>
     <row r="22">
@@ -677,7 +677,7 @@
         <v>43139</v>
       </c>
       <c r="C22" t="n">
-        <v>1.05113147631744</v>
+        <v>1.072975407245034</v>
       </c>
     </row>
     <row r="23">
@@ -688,7 +688,7 @@
         <v>43143</v>
       </c>
       <c r="C23" t="n">
-        <v>1.072085913516457</v>
+        <v>1.104339161454202</v>
       </c>
     </row>
     <row r="24">
@@ -699,7 +699,7 @@
         <v>43145</v>
       </c>
       <c r="C24" t="n">
-        <v>1.079355085319966</v>
+        <v>1.103672580710211</v>
       </c>
     </row>
     <row r="25">
@@ -710,7 +710,7 @@
         <v>43147</v>
       </c>
       <c r="C25" t="n">
-        <v>1.105429812869855</v>
+        <v>1.154173904746136</v>
       </c>
     </row>
     <row r="26">
@@ -721,7 +721,7 @@
         <v>43150</v>
       </c>
       <c r="C26" t="n">
-        <v>1.10550249227443</v>
+        <v>1.15397859907564</v>
       </c>
     </row>
     <row r="27">
@@ -732,7 +732,7 @@
         <v>43151</v>
       </c>
       <c r="C27" t="n">
-        <v>1.111224020493629</v>
+        <v>1.152275276538905</v>
       </c>
     </row>
     <row r="28">
@@ -743,7 +743,7 @@
         <v>43153</v>
       </c>
       <c r="C28" t="n">
-        <v>1.111257998375112</v>
+        <v>1.151101744275773</v>
       </c>
     </row>
     <row r="29">
@@ -754,7 +754,7 @@
         <v>43158</v>
       </c>
       <c r="C29" t="n">
-        <v>1.081019781323252</v>
+        <v>1.116782155375444</v>
       </c>
     </row>
     <row r="30">
@@ -765,7 +765,7 @@
         <v>43160</v>
       </c>
       <c r="C30" t="n">
-        <v>1.079668572299095</v>
+        <v>1.115048609808489</v>
       </c>
     </row>
     <row r="31">
@@ -776,7 +776,7 @@
         <v>43164</v>
       </c>
       <c r="C31" t="n">
-        <v>1.083834433885641</v>
+        <v>1.168912919956931</v>
       </c>
     </row>
     <row r="32">
@@ -787,7 +787,7 @@
         <v>43166</v>
       </c>
       <c r="C32" t="n">
-        <v>1.082309441064393</v>
+        <v>1.171086604455867</v>
       </c>
     </row>
     <row r="33">
@@ -798,7 +798,7 @@
         <v>43167</v>
       </c>
       <c r="C33" t="n">
-        <v>1.082854196019298</v>
+        <v>1.171537700052734</v>
       </c>
     </row>
     <row r="34">
@@ -809,7 +809,7 @@
         <v>43175</v>
       </c>
       <c r="C34" t="n">
-        <v>1.091136056435447</v>
+        <v>1.201170800994785</v>
       </c>
     </row>
     <row r="35">
@@ -820,7 +820,7 @@
         <v>43181</v>
       </c>
       <c r="C35" t="n">
-        <v>1.09107611317162</v>
+        <v>1.201128566809889</v>
       </c>
     </row>
     <row r="36">
@@ -831,7 +831,7 @@
         <v>43182</v>
       </c>
       <c r="C36" t="n">
-        <v>1.087798397901762</v>
+        <v>1.192348570778917</v>
       </c>
     </row>
     <row r="37">
@@ -842,7 +842,7 @@
         <v>43186</v>
       </c>
       <c r="C37" t="n">
-        <v>1.089714868823241</v>
+        <v>1.190544737130931</v>
       </c>
     </row>
     <row r="38">
@@ -853,7 +853,7 @@
         <v>43187</v>
       </c>
       <c r="C38" t="n">
-        <v>1.089577851118792</v>
+        <v>1.190402096186496</v>
       </c>
     </row>
     <row r="39">
@@ -864,7 +864,7 @@
         <v>43192</v>
       </c>
       <c r="C39" t="n">
-        <v>1.096809711857462</v>
+        <v>1.256585611518089</v>
       </c>
     </row>
     <row r="40">
@@ -875,7 +875,7 @@
         <v>43193</v>
       </c>
       <c r="C40" t="n">
-        <v>1.098126561236272</v>
+        <v>1.25645839590646</v>
       </c>
     </row>
     <row r="41">
@@ -886,7 +886,7 @@
         <v>43194</v>
       </c>
       <c r="C41" t="n">
-        <v>1.099008817648124</v>
+        <v>1.255591287367303</v>
       </c>
     </row>
     <row r="42">
@@ -897,7 +897,7 @@
         <v>43195</v>
       </c>
       <c r="C42" t="n">
-        <v>1.099641235900151</v>
+        <v>1.254472980603965</v>
       </c>
     </row>
     <row r="43">
@@ -908,7 +908,7 @@
         <v>43196</v>
       </c>
       <c r="C43" t="n">
-        <v>1.098615469088908</v>
+        <v>1.255731395696785</v>
       </c>
     </row>
     <row r="44">
@@ -919,7 +919,7 @@
         <v>43199</v>
       </c>
       <c r="C44" t="n">
-        <v>1.10080326926652</v>
+        <v>1.266271262789019</v>
       </c>
     </row>
     <row r="45">
@@ -930,7 +930,7 @@
         <v>43200</v>
       </c>
       <c r="C45" t="n">
-        <v>1.103435728833608</v>
+        <v>1.265851382956192</v>
       </c>
     </row>
     <row r="46">
@@ -941,7 +941,7 @@
         <v>43202</v>
       </c>
       <c r="C46" t="n">
-        <v>1.104295737942288</v>
+        <v>1.265827283350961</v>
       </c>
     </row>
     <row r="47">
@@ -952,7 +952,7 @@
         <v>43203</v>
       </c>
       <c r="C47" t="n">
-        <v>1.092818266674708</v>
+        <v>1.271937136825459</v>
       </c>
     </row>
     <row r="48">
@@ -963,7 +963,7 @@
         <v>43206</v>
       </c>
       <c r="C48" t="n">
-        <v>1.093397832901095</v>
+        <v>1.272467398213187</v>
       </c>
     </row>
     <row r="49">
@@ -974,7 +974,7 @@
         <v>43207</v>
       </c>
       <c r="C49" t="n">
-        <v>1.096522276137598</v>
+        <v>1.270812777561295</v>
       </c>
     </row>
     <row r="50">
@@ -985,7 +985,7 @@
         <v>43209</v>
       </c>
       <c r="C50" t="n">
-        <v>1.093183696421097</v>
+        <v>1.26176727629772</v>
       </c>
     </row>
     <row r="51">
@@ -996,7 +996,7 @@
         <v>43222</v>
       </c>
       <c r="C51" t="n">
-        <v>1.089328738934627</v>
+        <v>1.253784267928075</v>
       </c>
     </row>
     <row r="52">
@@ -1007,7 +1007,7 @@
         <v>43238</v>
       </c>
       <c r="C52" t="n">
-        <v>1.091866132460802</v>
+        <v>1.252765298039905</v>
       </c>
     </row>
     <row r="53">
@@ -1018,7 +1018,7 @@
         <v>43242</v>
       </c>
       <c r="C53" t="n">
-        <v>1.091555770708276</v>
+        <v>1.253123651328058</v>
       </c>
     </row>
     <row r="54">
@@ -1029,7 +1029,7 @@
         <v>43243</v>
       </c>
       <c r="C54" t="n">
-        <v>1.091473825263151</v>
+        <v>1.241437946494652</v>
       </c>
     </row>
     <row r="55">
@@ -1040,7 +1040,7 @@
         <v>43245</v>
       </c>
       <c r="C55" t="n">
-        <v>1.091757762787815</v>
+        <v>1.241440861519925</v>
       </c>
     </row>
     <row r="56">
@@ -1051,7 +1051,7 @@
         <v>43266</v>
       </c>
       <c r="C56" t="n">
-        <v>1.091425723368929</v>
+        <v>1.240964801001615</v>
       </c>
     </row>
     <row r="57">
@@ -1062,7 +1062,7 @@
         <v>43285</v>
       </c>
       <c r="C57" t="n">
-        <v>1.089011078721099</v>
+        <v>1.233023712212281</v>
       </c>
     </row>
     <row r="58">
@@ -1073,7 +1073,7 @@
         <v>43290</v>
       </c>
       <c r="C58" t="n">
-        <v>1.080135451193486</v>
+        <v>1.206762327715713</v>
       </c>
     </row>
     <row r="59">
@@ -1084,7 +1084,7 @@
         <v>43292</v>
       </c>
       <c r="C59" t="n">
-        <v>1.080112766372376</v>
+        <v>1.206345994313448</v>
       </c>
     </row>
     <row r="60">
@@ -1095,7 +1095,7 @@
         <v>43293</v>
       </c>
       <c r="C60" t="n">
-        <v>1.065850960921075</v>
+        <v>1.190363356309172</v>
       </c>
     </row>
     <row r="61">
@@ -1106,7 +1106,7 @@
         <v>43307</v>
       </c>
       <c r="C61" t="n">
-        <v>1.050159630062604</v>
+        <v>1.126567566400907</v>
       </c>
     </row>
     <row r="62">
@@ -1117,7 +1117,7 @@
         <v>43314</v>
       </c>
       <c r="C62" t="n">
-        <v>1.043789331814324</v>
+        <v>1.127425285703232</v>
       </c>
     </row>
     <row r="63">
@@ -1128,7 +1128,7 @@
         <v>43315</v>
       </c>
       <c r="C63" t="n">
-        <v>1.043918323990458</v>
+        <v>1.138242208322497</v>
       </c>
     </row>
     <row r="64">
@@ -1139,7 +1139,7 @@
         <v>43320</v>
       </c>
       <c r="C64" t="n">
-        <v>1.03319715593302</v>
+        <v>1.138449728405633</v>
       </c>
     </row>
     <row r="65">
@@ -1150,7 +1150,7 @@
         <v>43329</v>
       </c>
       <c r="C65" t="n">
-        <v>1.034887928252744</v>
+        <v>1.137061163458425</v>
       </c>
     </row>
     <row r="66">
@@ -1161,7 +1161,7 @@
         <v>43339</v>
       </c>
       <c r="C66" t="n">
-        <v>1.035114012314386</v>
+        <v>1.137263285609807</v>
       </c>
     </row>
     <row r="67">
@@ -1172,7 +1172,7 @@
         <v>43340</v>
       </c>
       <c r="C67" t="n">
-        <v>1.035085913842356</v>
+        <v>1.137378273119424</v>
       </c>
     </row>
     <row r="68">
@@ -1183,7 +1183,7 @@
         <v>43342</v>
       </c>
       <c r="C68" t="n">
-        <v>1.034632188504414</v>
+        <v>1.139834249723253</v>
       </c>
     </row>
     <row r="69">
@@ -1194,7 +1194,7 @@
         <v>43346</v>
       </c>
       <c r="C69" t="n">
-        <v>1.03490918991571</v>
+        <v>1.138910618196772</v>
       </c>
     </row>
     <row r="70">
@@ -1205,7 +1205,7 @@
         <v>43347</v>
       </c>
       <c r="C70" t="n">
-        <v>1.033863532989411</v>
+        <v>1.128750541746017</v>
       </c>
     </row>
     <row r="71">
@@ -1216,7 +1216,7 @@
         <v>43350</v>
       </c>
       <c r="C71" t="n">
-        <v>1.033339033171512</v>
+        <v>1.132720522804328</v>
       </c>
     </row>
     <row r="72">
@@ -1227,7 +1227,7 @@
         <v>43353</v>
       </c>
       <c r="C72" t="n">
-        <v>1.035201831434423</v>
+        <v>1.121011149323849</v>
       </c>
     </row>
     <row r="73">
@@ -1238,7 +1238,7 @@
         <v>43354</v>
       </c>
       <c r="C73" t="n">
-        <v>1.033902996755719</v>
+        <v>1.114359348770809</v>
       </c>
     </row>
     <row r="74">
@@ -1249,7 +1249,7 @@
         <v>43360</v>
       </c>
       <c r="C74" t="n">
-        <v>1.034011588261231</v>
+        <v>1.114335062412696</v>
       </c>
     </row>
     <row r="75">
@@ -1260,7 +1260,7 @@
         <v>43361</v>
       </c>
       <c r="C75" t="n">
-        <v>1.034034811354239</v>
+        <v>1.11425008567048</v>
       </c>
     </row>
     <row r="76">
@@ -1271,7 +1271,7 @@
         <v>43364</v>
       </c>
       <c r="C76" t="n">
-        <v>1.034196119105204</v>
+        <v>1.113899860711834</v>
       </c>
     </row>
     <row r="77">
@@ -1282,7 +1282,7 @@
         <v>43368</v>
       </c>
       <c r="C77" t="n">
-        <v>1.034456279163234</v>
+        <v>1.113275859222002</v>
       </c>
     </row>
     <row r="78">
@@ -1293,7 +1293,7 @@
         <v>43369</v>
       </c>
       <c r="C78" t="n">
-        <v>1.035228766191168</v>
+        <v>1.13541157614174</v>
       </c>
     </row>
     <row r="79">
@@ -1304,7 +1304,7 @@
         <v>43370</v>
       </c>
       <c r="C79" t="n">
-        <v>1.035803502003561</v>
+        <v>1.134249993198276</v>
       </c>
     </row>
     <row r="80">
@@ -1315,7 +1315,7 @@
         <v>43371</v>
       </c>
       <c r="C80" t="n">
-        <v>1.03734303966594</v>
+        <v>1.13244607182492</v>
       </c>
     </row>
     <row r="81">
@@ -1326,7 +1326,7 @@
         <v>43374</v>
       </c>
       <c r="C81" t="n">
-        <v>1.038683750536575</v>
+        <v>1.154468585366843</v>
       </c>
     </row>
     <row r="82">
@@ -1337,7 +1337,7 @@
         <v>43376</v>
       </c>
       <c r="C82" t="n">
-        <v>1.038650256109055</v>
+        <v>1.154133666960396</v>
       </c>
     </row>
     <row r="83">
@@ -1348,7 +1348,7 @@
         <v>43377</v>
       </c>
       <c r="C83" t="n">
-        <v>1.040318872693297</v>
+        <v>1.152131820219768</v>
       </c>
     </row>
     <row r="84">
@@ -1359,7 +1359,7 @@
         <v>43384</v>
       </c>
       <c r="C84" t="n">
-        <v>1.042387866281477</v>
+        <v>1.172039184262301</v>
       </c>
     </row>
     <row r="85">
@@ -1370,7 +1370,7 @@
         <v>43388</v>
       </c>
       <c r="C85" t="n">
-        <v>1.051123832979033</v>
+        <v>1.224331255543822</v>
       </c>
     </row>
     <row r="86">
@@ -1381,7 +1381,7 @@
         <v>43395</v>
       </c>
       <c r="C86" t="n">
-        <v>1.054553674687323</v>
+        <v>1.221224046685139</v>
       </c>
     </row>
     <row r="87">
@@ -1392,7 +1392,7 @@
         <v>43399</v>
       </c>
       <c r="C87" t="n">
-        <v>1.055527691913221</v>
+        <v>1.221676815557386</v>
       </c>
     </row>
     <row r="88">
@@ -1403,7 +1403,7 @@
         <v>43402</v>
       </c>
       <c r="C88" t="n">
-        <v>1.052258790963893</v>
+        <v>1.211803277145614</v>
       </c>
     </row>
     <row r="89">
@@ -1414,7 +1414,7 @@
         <v>43403</v>
       </c>
       <c r="C89" t="n">
-        <v>1.052554713281559</v>
+        <v>1.211473475788319</v>
       </c>
     </row>
     <row r="90">
@@ -1425,7 +1425,7 @@
         <v>43409</v>
       </c>
       <c r="C90" t="n">
-        <v>1.052713019770356</v>
+        <v>1.199342931175392</v>
       </c>
     </row>
     <row r="91">
@@ -1436,7 +1436,7 @@
         <v>43411</v>
       </c>
       <c r="C91" t="n">
-        <v>1.055841591470478</v>
+        <v>1.184069577065827</v>
       </c>
     </row>
     <row r="92">
@@ -1447,7 +1447,7 @@
         <v>43444</v>
       </c>
       <c r="C92" t="n">
-        <v>1.055309538694986</v>
+        <v>1.173905676291483</v>
       </c>
     </row>
     <row r="93">
@@ -1458,7 +1458,7 @@
         <v>43445</v>
       </c>
       <c r="C93" t="n">
-        <v>1.055223825110271</v>
+        <v>1.17385967852136</v>
       </c>
     </row>
     <row r="94">
@@ -1469,7 +1469,7 @@
         <v>43489</v>
       </c>
       <c r="C94" t="n">
-        <v>1.055342764969365</v>
+        <v>1.174830417757198</v>
       </c>
     </row>
     <row r="95">
@@ -1480,7 +1480,7 @@
         <v>43501</v>
       </c>
       <c r="C95" t="n">
-        <v>1.055901948044226</v>
+        <v>1.175729179955308</v>
       </c>
     </row>
     <row r="96">
@@ -1491,7 +1491,7 @@
         <v>43502</v>
       </c>
       <c r="C96" t="n">
-        <v>1.055405669987139</v>
+        <v>1.176404815787985</v>
       </c>
     </row>
     <row r="97">
@@ -1502,7 +1502,7 @@
         <v>43510</v>
       </c>
       <c r="C97" t="n">
-        <v>1.053745914909244</v>
+        <v>1.1665592742441</v>
       </c>
     </row>
     <row r="98">
@@ -1513,7 +1513,7 @@
         <v>43511</v>
       </c>
       <c r="C98" t="n">
-        <v>1.048979017110176</v>
+        <v>1.158572465294444</v>
       </c>
     </row>
     <row r="99">
@@ -1524,7 +1524,7 @@
         <v>43517</v>
       </c>
       <c r="C99" t="n">
-        <v>1.048995947256083</v>
+        <v>1.158973895104208</v>
       </c>
     </row>
     <row r="100">
@@ -1535,7 +1535,7 @@
         <v>43521</v>
       </c>
       <c r="C100" t="n">
-        <v>1.046152386914063</v>
+        <v>1.149632378146409</v>
       </c>
     </row>
     <row r="101">
@@ -1609,7 +1609,7 @@
         <v>43556</v>
       </c>
       <c r="C108" t="n">
-        <v>1.041528750125082</v>
+        <v>1.107940335399828</v>
       </c>
     </row>
     <row r="109">
@@ -1620,7 +1620,7 @@
         <v>43557</v>
       </c>
       <c r="C109" t="n">
-        <v>1.041563867344782</v>
+        <v>1.108060537129272</v>
       </c>
     </row>
     <row r="110">
@@ -1631,7 +1631,7 @@
         <v>43558</v>
       </c>
       <c r="C110" t="n">
-        <v>1.042327227701529</v>
+        <v>1.107370119993902</v>
       </c>
     </row>
     <row r="111">
@@ -1642,7 +1642,7 @@
         <v>43560</v>
       </c>
       <c r="C111" t="n">
-        <v>1.042813005632781</v>
+        <v>1.106542397422774</v>
       </c>
     </row>
     <row r="112">
@@ -1653,7 +1653,7 @@
         <v>43565</v>
       </c>
       <c r="C112" t="n">
-        <v>1.043411989098391</v>
+        <v>1.105493868205267</v>
       </c>
     </row>
     <row r="113">
@@ -1664,7 +1664,7 @@
         <v>43567</v>
       </c>
       <c r="C113" t="n">
-        <v>1.042729768008423</v>
+        <v>1.105125707572036</v>
       </c>
     </row>
     <row r="114">
@@ -1675,7 +1675,7 @@
         <v>43570</v>
       </c>
       <c r="C114" t="n">
-        <v>1.043565915253684</v>
+        <v>1.115068499795452</v>
       </c>
     </row>
     <row r="115">
@@ -1686,7 +1686,7 @@
         <v>43571</v>
       </c>
       <c r="C115" t="n">
-        <v>1.04447519122487</v>
+        <v>1.114254831892714</v>
       </c>
     </row>
     <row r="116">
@@ -1697,7 +1697,7 @@
         <v>43573</v>
       </c>
       <c r="C116" t="n">
-        <v>1.045881227360774</v>
+        <v>1.112856113602457</v>
       </c>
     </row>
     <row r="117">
@@ -1708,7 +1708,7 @@
         <v>43577</v>
       </c>
       <c r="C117" t="n">
-        <v>1.046781068952759</v>
+        <v>1.112475140268308</v>
       </c>
     </row>
     <row r="118">
@@ -1719,7 +1719,7 @@
         <v>43581</v>
       </c>
       <c r="C118" t="n">
-        <v>1.047315236400072</v>
+        <v>1.112209087446224</v>
       </c>
     </row>
     <row r="119">
@@ -1730,7 +1730,7 @@
         <v>43642</v>
       </c>
       <c r="C119" t="n">
-        <v>1.045384919370431</v>
+        <v>1.1161820754139</v>
       </c>
     </row>
     <row r="120">
@@ -1741,7 +1741,7 @@
         <v>43655</v>
       </c>
       <c r="C120" t="n">
-        <v>1.046158594481304</v>
+        <v>1.126941622960825</v>
       </c>
     </row>
     <row r="121">
@@ -1752,7 +1752,7 @@
         <v>43658</v>
       </c>
       <c r="C121" t="n">
-        <v>1.046164758789224</v>
+        <v>1.126843444674365</v>
       </c>
     </row>
     <row r="122">
@@ -1763,7 +1763,7 @@
         <v>43665</v>
       </c>
       <c r="C122" t="n">
-        <v>1.046353107935187</v>
+        <v>1.127463979637</v>
       </c>
     </row>
     <row r="123">
@@ -1774,7 +1774,7 @@
         <v>43671</v>
       </c>
       <c r="C123" t="n">
-        <v>1.047593699407971</v>
+        <v>1.126174461019056</v>
       </c>
     </row>
     <row r="124">
@@ -1785,7 +1785,7 @@
         <v>43684</v>
       </c>
       <c r="C124" t="n">
-        <v>1.046573093171695</v>
+        <v>1.138381876588213</v>
       </c>
     </row>
     <row r="125">
@@ -1796,7 +1796,7 @@
         <v>43686</v>
       </c>
       <c r="C125" t="n">
-        <v>1.046822522829834</v>
+        <v>1.13806908858605</v>
       </c>
     </row>
     <row r="126">
@@ -1807,7 +1807,7 @@
         <v>43698</v>
       </c>
       <c r="C126" t="n">
-        <v>1.04814881663439</v>
+        <v>1.137109359129242</v>
       </c>
     </row>
     <row r="127">
@@ -1818,7 +1818,7 @@
         <v>43713</v>
       </c>
       <c r="C127" t="n">
-        <v>1.048086374193081</v>
+        <v>1.137315445642634</v>
       </c>
     </row>
     <row r="128">
@@ -1829,7 +1829,7 @@
         <v>43725</v>
       </c>
       <c r="C128" t="n">
-        <v>1.049922845279386</v>
+        <v>1.133996296762787</v>
       </c>
     </row>
     <row r="129">
@@ -1840,7 +1840,7 @@
         <v>43727</v>
       </c>
       <c r="C129" t="n">
-        <v>1.049400551234431</v>
+        <v>1.134295282543967</v>
       </c>
     </row>
     <row r="130">
@@ -1851,7 +1851,7 @@
         <v>43728</v>
       </c>
       <c r="C130" t="n">
-        <v>1.049016345979472</v>
+        <v>1.124155135788364</v>
       </c>
     </row>
     <row r="131">
@@ -1862,7 +1862,7 @@
         <v>43732</v>
       </c>
       <c r="C131" t="n">
-        <v>1.049845411015274</v>
+        <v>1.157925021332974</v>
       </c>
     </row>
     <row r="132">
@@ -1873,7 +1873,7 @@
         <v>43745</v>
       </c>
       <c r="C132" t="n">
-        <v>1.051901300088614</v>
+        <v>1.158999694206957</v>
       </c>
     </row>
     <row r="133">
@@ -1884,7 +1884,7 @@
         <v>43748</v>
       </c>
       <c r="C133" t="n">
-        <v>1.051428393664892</v>
+        <v>1.16055193328042</v>
       </c>
     </row>
     <row r="134">
@@ -1895,7 +1895,7 @@
         <v>43765</v>
       </c>
       <c r="C134" t="n">
-        <v>1.052941609626039</v>
+        <v>1.160146352695709</v>
       </c>
     </row>
     <row r="135">
@@ -1906,7 +1906,7 @@
         <v>43767</v>
       </c>
       <c r="C135" t="n">
-        <v>1.053305830523551</v>
+        <v>1.159970400536639</v>
       </c>
     </row>
     <row r="136">
@@ -1917,7 +1917,7 @@
         <v>43769</v>
       </c>
       <c r="C136" t="n">
-        <v>1.048447326557774</v>
+        <v>1.141695664908062</v>
       </c>
     </row>
     <row r="137">
@@ -1928,7 +1928,7 @@
         <v>43770</v>
       </c>
       <c r="C137" t="n">
-        <v>1.049890549212762</v>
+        <v>1.14019684256831</v>
       </c>
     </row>
     <row r="138">
@@ -1939,7 +1939,7 @@
         <v>43773</v>
       </c>
       <c r="C138" t="n">
-        <v>1.050963325410521</v>
+        <v>1.139070158447221</v>
       </c>
     </row>
     <row r="139">
@@ -1950,7 +1950,7 @@
         <v>43774</v>
       </c>
       <c r="C139" t="n">
-        <v>1.05126872997379</v>
+        <v>1.138445041950447</v>
       </c>
     </row>
     <row r="140">
@@ -1961,7 +1961,7 @@
         <v>43780</v>
       </c>
       <c r="C140" t="n">
-        <v>1.050742563081493</v>
+        <v>1.12740910256125</v>
       </c>
     </row>
     <row r="141">
@@ -1972,7 +1972,7 @@
         <v>43791</v>
       </c>
       <c r="C141" t="n">
-        <v>1.042381609725417</v>
+        <v>1.111055506179252</v>
       </c>
     </row>
     <row r="142">
@@ -1983,7 +1983,7 @@
         <v>43794</v>
       </c>
       <c r="C142" t="n">
-        <v>1.042787959840901</v>
+        <v>1.133181063208494</v>
       </c>
     </row>
     <row r="143">
@@ -1994,7 +1994,7 @@
         <v>43797</v>
       </c>
       <c r="C143" t="n">
-        <v>1.051734565201219</v>
+        <v>1.150064950066143</v>
       </c>
     </row>
     <row r="144">
@@ -2005,7 +2005,7 @@
         <v>43822</v>
       </c>
       <c r="C144" t="n">
-        <v>1.053426257800849</v>
+        <v>1.160586009022143</v>
       </c>
     </row>
     <row r="145">
@@ -2016,7 +2016,7 @@
         <v>43826</v>
       </c>
       <c r="C145" t="n">
-        <v>1.054102075596851</v>
+        <v>1.171993481850155</v>
       </c>
     </row>
     <row r="146">
@@ -2027,7 +2027,7 @@
         <v>43833</v>
       </c>
       <c r="C146" t="n">
-        <v>1.056144365894703</v>
+        <v>1.183431398467235</v>
       </c>
     </row>
     <row r="147">
@@ -2038,7 +2038,7 @@
         <v>43836</v>
       </c>
       <c r="C147" t="n">
-        <v>1.058158292102837</v>
+        <v>1.218056825832585</v>
       </c>
     </row>
     <row r="148">
@@ -2049,7 +2049,7 @@
         <v>43840</v>
       </c>
       <c r="C148" t="n">
-        <v>1.059800334232079</v>
+        <v>1.279280605515099</v>
       </c>
     </row>
     <row r="149">
@@ -2060,7 +2060,7 @@
         <v>43844</v>
       </c>
       <c r="C149" t="n">
-        <v>1.058199863189048</v>
+        <v>1.229123295592256</v>
       </c>
     </row>
     <row r="150">
@@ -2071,7 +2071,7 @@
         <v>43851</v>
       </c>
       <c r="C150" t="n">
-        <v>1.05984283021177</v>
+        <v>1.227137682520593</v>
       </c>
     </row>
     <row r="151">
@@ -2082,7 +2082,7 @@
         <v>43858</v>
       </c>
       <c r="C151" t="n">
-        <v>1.061159645732337</v>
+        <v>1.246933913732589</v>
       </c>
     </row>
     <row r="152">
@@ -2093,7 +2093,7 @@
         <v>43862</v>
       </c>
       <c r="C152" t="n">
-        <v>1.060547133637636</v>
+        <v>1.23607283366597</v>
       </c>
     </row>
     <row r="153">
@@ -2104,7 +2104,7 @@
         <v>43864</v>
       </c>
       <c r="C153" t="n">
-        <v>1.060434394167634</v>
+        <v>1.224823220785524</v>
       </c>
     </row>
     <row r="154">
@@ -2115,7 +2115,7 @@
         <v>43866</v>
       </c>
       <c r="C154" t="n">
-        <v>1.060052683506216</v>
+        <v>1.226944694179454</v>
       </c>
     </row>
     <row r="155">
@@ -2126,7 +2126,7 @@
         <v>43868</v>
       </c>
       <c r="C155" t="n">
-        <v>1.061165877296597</v>
+        <v>1.251906424361683</v>
       </c>
     </row>
     <row r="156">
@@ -2137,7 +2137,7 @@
         <v>43871</v>
       </c>
       <c r="C156" t="n">
-        <v>1.060925276090412</v>
+        <v>1.237614583432442</v>
       </c>
     </row>
     <row r="157">
@@ -2148,7 +2148,7 @@
         <v>43874</v>
       </c>
       <c r="C157" t="n">
-        <v>1.055358706350573</v>
+        <v>1.229252052756492</v>
       </c>
     </row>
     <row r="158">
@@ -2159,7 +2159,7 @@
         <v>43878</v>
       </c>
       <c r="C158" t="n">
-        <v>1.058615388708072</v>
+        <v>1.22837241215929</v>
       </c>
     </row>
     <row r="159">
@@ -2170,7 +2170,7 @@
         <v>43894</v>
       </c>
       <c r="C159" t="n">
-        <v>1.060900434851139</v>
+        <v>1.224836949211642</v>
       </c>
     </row>
     <row r="160">
@@ -2181,7 +2181,7 @@
         <v>43896</v>
       </c>
       <c r="C160" t="n">
-        <v>1.060768392132715</v>
+        <v>1.224984431986622</v>
       </c>
     </row>
     <row r="161">
@@ -2192,7 +2192,7 @@
         <v>43903</v>
       </c>
       <c r="C161" t="n">
-        <v>1.064070115542181</v>
+        <v>1.236011763862107</v>
       </c>
     </row>
     <row r="162">
@@ -2203,7 +2203,7 @@
         <v>43906</v>
       </c>
       <c r="C162" t="n">
-        <v>1.051559554651461</v>
+        <v>1.207591852601023</v>
       </c>
     </row>
     <row r="163">
@@ -2214,7 +2214,7 @@
         <v>43907</v>
       </c>
       <c r="C163" t="n">
-        <v>1.054571485152438</v>
+        <v>1.230794649035045</v>
       </c>
     </row>
     <row r="164">
@@ -2225,7 +2225,7 @@
         <v>43908</v>
       </c>
       <c r="C164" t="n">
-        <v>1.0738304186006</v>
+        <v>1.221684457077438</v>
       </c>
     </row>
     <row r="165">
@@ -2236,7 +2236,7 @@
         <v>43909</v>
       </c>
       <c r="C165" t="n">
-        <v>1.075398698495341</v>
+        <v>1.220835698303138</v>
       </c>
     </row>
     <row r="166">
@@ -2247,7 +2247,7 @@
         <v>43910</v>
       </c>
       <c r="C166" t="n">
-        <v>1.077243336758605</v>
+        <v>1.232434072515213</v>
       </c>
     </row>
     <row r="167">
@@ -2258,7 +2258,7 @@
         <v>43915</v>
       </c>
       <c r="C167" t="n">
-        <v>1.079295375549931</v>
+        <v>1.254963830814965</v>
       </c>
     </row>
     <row r="168">
@@ -2269,7 +2269,7 @@
         <v>43916</v>
       </c>
       <c r="C168" t="n">
-        <v>1.078882327785265</v>
+        <v>1.255495348108507</v>
       </c>
     </row>
     <row r="169">
@@ -2280,7 +2280,7 @@
         <v>43917</v>
       </c>
       <c r="C169" t="n">
-        <v>1.083270669361097</v>
+        <v>1.2534346438466</v>
       </c>
     </row>
     <row r="170">
@@ -2291,7 +2291,7 @@
         <v>43924</v>
       </c>
       <c r="C170" t="n">
-        <v>1.088104164494333</v>
+        <v>1.254367011593912</v>
       </c>
     </row>
     <row r="171">
@@ -2302,7 +2302,7 @@
         <v>43936</v>
       </c>
       <c r="C171" t="n">
-        <v>1.092730356330316</v>
+        <v>1.244902103092612</v>
       </c>
     </row>
     <row r="172">
@@ -2313,7 +2313,7 @@
         <v>43942</v>
       </c>
       <c r="C172" t="n">
-        <v>1.094956742886887</v>
+        <v>1.241195847876235</v>
       </c>
     </row>
     <row r="173">
@@ -2324,7 +2324,7 @@
         <v>43944</v>
       </c>
       <c r="C173" t="n">
-        <v>1.096484227872294</v>
+        <v>1.261512601196585</v>
       </c>
     </row>
     <row r="174">
@@ -2335,7 +2335,7 @@
         <v>43978</v>
       </c>
       <c r="C174" t="n">
-        <v>1.103816796938806</v>
+        <v>1.261262648244235</v>
       </c>
     </row>
     <row r="175">
@@ -2346,7 +2346,7 @@
         <v>43984</v>
       </c>
       <c r="C175" t="n">
-        <v>1.099040436558271</v>
+        <v>1.261336298305191</v>
       </c>
     </row>
     <row r="176">
@@ -2357,7 +2357,7 @@
         <v>43987</v>
       </c>
       <c r="C176" t="n">
-        <v>1.090855208800219</v>
+        <v>1.249861813975672</v>
       </c>
     </row>
     <row r="177">
@@ -2368,7 +2368,7 @@
         <v>43990</v>
       </c>
       <c r="C177" t="n">
-        <v>1.091230457234189</v>
+        <v>1.240033735009614</v>
       </c>
     </row>
     <row r="178">
@@ -2379,7 +2379,7 @@
         <v>43993</v>
       </c>
       <c r="C178" t="n">
-        <v>1.094652945333106</v>
+        <v>1.239394757491263</v>
       </c>
     </row>
     <row r="179">
@@ -2390,7 +2390,7 @@
         <v>43994</v>
       </c>
       <c r="C179" t="n">
-        <v>1.094798901730876</v>
+        <v>1.23954558693412</v>
       </c>
     </row>
     <row r="180">
@@ -2401,7 +2401,7 @@
         <v>44012</v>
       </c>
       <c r="C180" t="n">
-        <v>1.0942821616358</v>
+        <v>1.251983199626977</v>
       </c>
     </row>
     <row r="181">
@@ -2412,7 +2412,7 @@
         <v>44018</v>
       </c>
       <c r="C181" t="n">
-        <v>1.091262307033655</v>
+        <v>1.241037469156476</v>
       </c>
     </row>
     <row r="182">
@@ -2423,7 +2423,7 @@
         <v>44019</v>
       </c>
       <c r="C182" t="n">
-        <v>1.091903074566645</v>
+        <v>1.242260237272236</v>
       </c>
     </row>
     <row r="183">
@@ -2434,7 +2434,7 @@
         <v>44025</v>
       </c>
       <c r="C183" t="n">
-        <v>1.092167220762358</v>
+        <v>1.23127665903962</v>
       </c>
     </row>
     <row r="184">
@@ -2445,7 +2445,7 @@
         <v>44036</v>
       </c>
       <c r="C184" t="n">
-        <v>1.091183708815661</v>
+        <v>1.241476453272779</v>
       </c>
     </row>
     <row r="185">
@@ -2456,7 +2456,7 @@
         <v>44039</v>
       </c>
       <c r="C185" t="n">
-        <v>1.092986564787755</v>
+        <v>1.229237977219085</v>
       </c>
     </row>
     <row r="186">
@@ -2467,7 +2467,7 @@
         <v>44055</v>
       </c>
       <c r="C186" t="n">
-        <v>1.093367883797541</v>
+        <v>1.239780167189877</v>
       </c>
     </row>
     <row r="187">
@@ -2478,7 +2478,7 @@
         <v>44064</v>
       </c>
       <c r="C187" t="n">
-        <v>1.092180741324223</v>
+        <v>1.226584416410468</v>
       </c>
     </row>
     <row r="188">
@@ -2489,7 +2489,7 @@
         <v>44067</v>
       </c>
       <c r="C188" t="n">
-        <v>1.092282015479355</v>
+        <v>1.2271120409947</v>
       </c>
     </row>
     <row r="189">
@@ -2500,7 +2500,7 @@
         <v>44085</v>
       </c>
       <c r="C189" t="n">
-        <v>1.095178287548424</v>
+        <v>1.216585938746457</v>
       </c>
     </row>
     <row r="190">
@@ -2511,7 +2511,7 @@
         <v>44088</v>
       </c>
       <c r="C190" t="n">
-        <v>1.085309757724072</v>
+        <v>1.205855239162779</v>
       </c>
     </row>
     <row r="191">
@@ -2522,7 +2522,7 @@
         <v>44095</v>
       </c>
       <c r="C191" t="n">
-        <v>1.086706042642213</v>
+        <v>1.217026667395232</v>
       </c>
     </row>
     <row r="192">
@@ -2533,7 +2533,7 @@
         <v>44097</v>
       </c>
       <c r="C192" t="n">
-        <v>1.089162156627261</v>
+        <v>1.215240278202451</v>
       </c>
     </row>
     <row r="193">
@@ -2544,7 +2544,7 @@
         <v>44098</v>
       </c>
       <c r="C193" t="n">
-        <v>1.091149045163861</v>
+        <v>1.227180250068359</v>
       </c>
     </row>
     <row r="194">
@@ -2555,7 +2555,7 @@
         <v>44119</v>
       </c>
       <c r="C194" t="n">
-        <v>1.091727984875611</v>
+        <v>1.215312874015924</v>
       </c>
     </row>
     <row r="195">
@@ -2566,7 +2566,7 @@
         <v>44145</v>
       </c>
       <c r="C195" t="n">
-        <v>1.083551791462283</v>
+        <v>1.202205697756833</v>
       </c>
     </row>
     <row r="196">
@@ -2577,7 +2577,7 @@
         <v>44146</v>
       </c>
       <c r="C196" t="n">
-        <v>1.084356493757403</v>
+        <v>1.201632555334657</v>
       </c>
     </row>
     <row r="197">
@@ -2588,7 +2588,7 @@
         <v>44149</v>
       </c>
       <c r="C197" t="n">
-        <v>1.086200592925574</v>
+        <v>1.200778399893643</v>
       </c>
     </row>
     <row r="198">
@@ -2599,7 +2599,7 @@
         <v>44155</v>
       </c>
       <c r="C198" t="n">
-        <v>1.085822373538622</v>
+        <v>1.201464048788146</v>
       </c>
     </row>
     <row r="199">
@@ -2610,7 +2610,7 @@
         <v>44158</v>
       </c>
       <c r="C199" t="n">
-        <v>1.081519609469212</v>
+        <v>1.183154368829215</v>
       </c>
     </row>
     <row r="200">
@@ -2621,7 +2621,7 @@
         <v>44159</v>
       </c>
       <c r="C200" t="n">
-        <v>1.081682382595151</v>
+        <v>1.183031700089795</v>
       </c>
     </row>
     <row r="201">
@@ -2632,7 +2632,7 @@
         <v>44160</v>
       </c>
       <c r="C201" t="n">
-        <v>1.092369505623297</v>
+        <v>1.13456643813505</v>
       </c>
     </row>
     <row r="202">
@@ -2643,7 +2643,7 @@
         <v>44161</v>
       </c>
       <c r="C202" t="n">
-        <v>1.107480011915043</v>
+        <v>1.156068047470161</v>
       </c>
     </row>
     <row r="203">
@@ -2654,7 +2654,7 @@
         <v>44162</v>
       </c>
       <c r="C203" t="n">
-        <v>1.110643175830219</v>
+        <v>1.155501233956457</v>
       </c>
     </row>
     <row r="204">
@@ -2665,7 +2665,7 @@
         <v>44181</v>
       </c>
       <c r="C204" t="n">
-        <v>1.121146425298121</v>
+        <v>1.15857937289105</v>
       </c>
     </row>
     <row r="205">
@@ -2676,7 +2676,7 @@
         <v>44182</v>
       </c>
       <c r="C205" t="n">
-        <v>1.122934680368068</v>
+        <v>1.15887324167878</v>
       </c>
     </row>
     <row r="206">
@@ -2687,7 +2687,7 @@
         <v>44186</v>
       </c>
       <c r="C206" t="n">
-        <v>1.124924628192205</v>
+        <v>1.160518084841505</v>
       </c>
     </row>
     <row r="207">
@@ -2698,7 +2698,7 @@
         <v>44189</v>
       </c>
       <c r="C207" t="n">
-        <v>1.126319659496966</v>
+        <v>1.15848941299581</v>
       </c>
     </row>
     <row r="208">
@@ -2709,7 +2709,7 @@
         <v>44194</v>
       </c>
       <c r="C208" t="n">
-        <v>1.125099131562083</v>
+        <v>1.157727480446831</v>
       </c>
     </row>
     <row r="209">
@@ -2720,7 +2720,7 @@
         <v>44196</v>
       </c>
       <c r="C209" t="n">
-        <v>1.137037719603685</v>
+        <v>1.198382104895903</v>
       </c>
     </row>
     <row r="210">
@@ -2731,7 +2731,7 @@
         <v>44197</v>
       </c>
       <c r="C210" t="n">
-        <v>1.139008400611342</v>
+        <v>1.195773103512876</v>
       </c>
     </row>
     <row r="211">
@@ -2742,7 +2742,7 @@
         <v>44200</v>
       </c>
       <c r="C211" t="n">
-        <v>1.138629444931291</v>
+        <v>1.209974452832892</v>
       </c>
     </row>
     <row r="212">
@@ -2753,7 +2753,7 @@
         <v>44203</v>
       </c>
       <c r="C212" t="n">
-        <v>1.138636581696853</v>
+        <v>1.208331063335448</v>
       </c>
     </row>
     <row r="213">
@@ -2764,7 +2764,7 @@
         <v>44209</v>
       </c>
       <c r="C213" t="n">
-        <v>1.13893354673652</v>
+        <v>1.189155755876344</v>
       </c>
     </row>
     <row r="214">
@@ -2775,7 +2775,7 @@
         <v>44236</v>
       </c>
       <c r="C214" t="n">
-        <v>1.141190341254279</v>
+        <v>1.202454954866687</v>
       </c>
     </row>
     <row r="215">
@@ -2786,7 +2786,7 @@
         <v>44244</v>
       </c>
       <c r="C215" t="n">
-        <v>1.144764275890759</v>
+        <v>1.229650274417446</v>
       </c>
     </row>
     <row r="216">
@@ -2797,7 +2797,7 @@
         <v>44246</v>
       </c>
       <c r="C216" t="n">
-        <v>1.146285936654774</v>
+        <v>1.25238777795289</v>
       </c>
     </row>
     <row r="217">
@@ -2808,7 +2808,7 @@
         <v>44252</v>
       </c>
       <c r="C217" t="n">
-        <v>1.148549761344456</v>
+        <v>1.263602360411059</v>
       </c>
     </row>
     <row r="218">
@@ -2819,7 +2819,7 @@
         <v>44253</v>
       </c>
       <c r="C218" t="n">
-        <v>1.147854443184673</v>
+        <v>1.246387192911335</v>
       </c>
     </row>
     <row r="219">
@@ -2830,7 +2830,7 @@
         <v>44258</v>
       </c>
       <c r="C219" t="n">
-        <v>1.149151585674543</v>
+        <v>1.264182301588832</v>
       </c>
     </row>
     <row r="220">
@@ -2841,7 +2841,7 @@
         <v>44259</v>
       </c>
       <c r="C220" t="n">
-        <v>1.15114754770312</v>
+        <v>1.263848875603399</v>
       </c>
     </row>
     <row r="221">
@@ -2852,7 +2852,7 @@
         <v>44271</v>
       </c>
       <c r="C221" t="n">
-        <v>1.151449920908787</v>
+        <v>1.246523043307328</v>
       </c>
     </row>
     <row r="222">
@@ -2863,7 +2863,7 @@
         <v>44272</v>
       </c>
       <c r="C222" t="n">
-        <v>1.150996176280462</v>
+        <v>1.263996964619386</v>
       </c>
     </row>
     <row r="223">
@@ -2874,7 +2874,7 @@
         <v>44278</v>
       </c>
       <c r="C223" t="n">
-        <v>1.14814556987971</v>
+        <v>1.261754686587591</v>
       </c>
     </row>
     <row r="224">
@@ -2885,7 +2885,7 @@
         <v>44279</v>
       </c>
       <c r="C224" t="n">
-        <v>1.15115028093396</v>
+        <v>1.27569387525055</v>
       </c>
     </row>
     <row r="225">
@@ -2896,7 +2896,7 @@
         <v>44285</v>
       </c>
       <c r="C225" t="n">
-        <v>1.134899864986688</v>
+        <v>1.22545551860092</v>
       </c>
     </row>
     <row r="226">
@@ -2907,7 +2907,7 @@
         <v>44286</v>
       </c>
       <c r="C226" t="n">
-        <v>1.134453848702452</v>
+        <v>1.225199638967192</v>
       </c>
     </row>
     <row r="227">
@@ -2918,7 +2918,7 @@
         <v>44287</v>
       </c>
       <c r="C227" t="n">
-        <v>1.134876838072908</v>
+        <v>1.224741771886805</v>
       </c>
     </row>
     <row r="228">
@@ -2929,7 +2929,7 @@
         <v>44295</v>
       </c>
       <c r="C228" t="n">
-        <v>1.134680803962864</v>
+        <v>1.236066745689059</v>
       </c>
     </row>
     <row r="229">
@@ -2940,7 +2940,7 @@
         <v>44298</v>
       </c>
       <c r="C229" t="n">
-        <v>1.125747199536143</v>
+        <v>1.210369893739896</v>
       </c>
     </row>
     <row r="230">
@@ -2951,7 +2951,7 @@
         <v>44301</v>
       </c>
       <c r="C230" t="n">
-        <v>1.136883885438468</v>
+        <v>1.220969765170798</v>
       </c>
     </row>
     <row r="231">
@@ -2962,7 +2962,7 @@
         <v>44302</v>
       </c>
       <c r="C231" t="n">
-        <v>1.137216306745685</v>
+        <v>1.209418120636799</v>
       </c>
     </row>
     <row r="232">
@@ -2973,7 +2973,7 @@
         <v>44305</v>
       </c>
       <c r="C232" t="n">
-        <v>1.13821556794006</v>
+        <v>1.231913282552143</v>
       </c>
     </row>
     <row r="233">
@@ -2984,7 +2984,7 @@
         <v>44308</v>
       </c>
       <c r="C233" t="n">
-        <v>1.138865654884769</v>
+        <v>1.207602739803586</v>
       </c>
     </row>
     <row r="234">
@@ -2995,7 +2995,7 @@
         <v>44313</v>
       </c>
       <c r="C234" t="n">
-        <v>1.140038263631865</v>
+        <v>1.255041069324126</v>
       </c>
     </row>
     <row r="235">
@@ -3006,7 +3006,7 @@
         <v>44316</v>
       </c>
       <c r="C235" t="n">
-        <v>1.142023555242022</v>
+        <v>1.254195005234185</v>
       </c>
     </row>
     <row r="236">
@@ -3017,7 +3017,7 @@
         <v>44319</v>
       </c>
       <c r="C236" t="n">
-        <v>1.143329467856315</v>
+        <v>1.252772036376002</v>
       </c>
     </row>
     <row r="237">
@@ -3028,7 +3028,7 @@
         <v>44320</v>
       </c>
       <c r="C237" t="n">
-        <v>1.143714651512444</v>
+        <v>1.252042889877839</v>
       </c>
     </row>
     <row r="238">
@@ -3039,7 +3039,7 @@
         <v>44321</v>
       </c>
       <c r="C238" t="n">
-        <v>1.143628613016194</v>
+        <v>1.251956762518444</v>
       </c>
     </row>
     <row r="239">
@@ -3050,7 +3050,7 @@
         <v>44323</v>
       </c>
       <c r="C239" t="n">
-        <v>1.144010981413483</v>
+        <v>1.251751250277681</v>
       </c>
     </row>
     <row r="240">
@@ -3061,7 +3061,7 @@
         <v>44326</v>
       </c>
       <c r="C240" t="n">
-        <v>1.147463588741738</v>
+        <v>1.2874931684436</v>
       </c>
     </row>
     <row r="241">
@@ -3072,7 +3072,7 @@
         <v>44327</v>
       </c>
       <c r="C241" t="n">
-        <v>1.147674934819676</v>
+        <v>1.286762522544962</v>
       </c>
     </row>
     <row r="242">
@@ -3083,7 +3083,7 @@
         <v>44330</v>
       </c>
       <c r="C242" t="n">
-        <v>1.125451351306907</v>
+        <v>1.274961369456642</v>
       </c>
     </row>
     <row r="243">
@@ -3094,7 +3094,7 @@
         <v>44333</v>
       </c>
       <c r="C243" t="n">
-        <v>1.149147151898669</v>
+        <v>1.300049538884881</v>
       </c>
     </row>
     <row r="244">
@@ -3105,7 +3105,7 @@
         <v>44334</v>
       </c>
       <c r="C244" t="n">
-        <v>1.152113481421156</v>
+        <v>1.338039754440691</v>
       </c>
     </row>
     <row r="245">
@@ -3116,7 +3116,7 @@
         <v>44335</v>
       </c>
       <c r="C245" t="n">
-        <v>1.153142134887924</v>
+        <v>1.374859519035824</v>
       </c>
     </row>
     <row r="246">
@@ -3126,9 +3126,7 @@
       <c r="B246" s="2" t="n">
         <v>44336</v>
       </c>
-      <c r="C246" t="n">
-        <v>1.156008252672189</v>
-      </c>
+      <c r="C246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -3138,7 +3136,7 @@
         <v>44337</v>
       </c>
       <c r="C247" t="n">
-        <v>1.158833936714113</v>
+        <v>1.371693481153703</v>
       </c>
     </row>
     <row r="248">
@@ -3148,9 +3146,7 @@
       <c r="B248" s="2" t="n">
         <v>44340</v>
       </c>
-      <c r="C248" t="n">
-        <v>1.160652797704466</v>
-      </c>
+      <c r="C248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -3159,9 +3155,7 @@
       <c r="B249" s="2" t="n">
         <v>44341</v>
       </c>
-      <c r="C249" t="n">
-        <v>1.164688864978861</v>
-      </c>
+      <c r="C249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -3170,9 +3164,7 @@
       <c r="B250" s="2" t="n">
         <v>44343</v>
       </c>
-      <c r="C250" t="n">
-        <v>1.166672403733199</v>
-      </c>
+      <c r="C250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -3182,7 +3174,7 @@
         <v>44347</v>
       </c>
       <c r="C251" t="n">
-        <v>1.169210683095488</v>
+        <v>1.519169109159574</v>
       </c>
     </row>
     <row r="252">
@@ -3193,7 +3185,7 @@
         <v>44348</v>
       </c>
       <c r="C252" t="n">
-        <v>1.168210345124246</v>
+        <v>1.474518038152608</v>
       </c>
     </row>
     <row r="253">
@@ -3204,7 +3196,7 @@
         <v>44349</v>
       </c>
       <c r="C253" t="n">
-        <v>1.169796420943737</v>
+        <v>1.504288327170114</v>
       </c>
     </row>
     <row r="254">
@@ -3215,7 +3207,7 @@
         <v>44351</v>
       </c>
       <c r="C254" t="n">
-        <v>1.175402073082716</v>
+        <v>1.466625075063962</v>
       </c>
     </row>
     <row r="255">
@@ -3226,7 +3218,7 @@
         <v>44355</v>
       </c>
       <c r="C255" t="n">
-        <v>1.185630501623239</v>
+        <v>1.487414744654503</v>
       </c>
     </row>
     <row r="256">
@@ -3237,7 +3229,7 @@
         <v>44357</v>
       </c>
       <c r="C256" t="n">
-        <v>1.186254073439</v>
+        <v>1.488487519902972</v>
       </c>
     </row>
     <row r="257">
@@ -3248,7 +3240,7 @@
         <v>44362</v>
       </c>
       <c r="C257" t="n">
-        <v>1.188487881926738</v>
+        <v>1.529535266598068</v>
       </c>
     </row>
     <row r="258">
@@ -3259,7 +3251,7 @@
         <v>44364</v>
       </c>
       <c r="C258" t="n">
-        <v>1.188059253219818</v>
+        <v>1.528304800455153</v>
       </c>
     </row>
     <row r="259">
@@ -3269,9 +3261,7 @@
       <c r="B259" s="2" t="n">
         <v>44365</v>
       </c>
-      <c r="C259" t="n">
-        <v>1.187270915729757</v>
-      </c>
+      <c r="C259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -3281,7 +3271,7 @@
         <v>44369</v>
       </c>
       <c r="C260" t="n">
-        <v>1.183369384577944</v>
+        <v>1.488052452559537</v>
       </c>
     </row>
     <row r="261">
@@ -3291,9 +3281,7 @@
       <c r="B261" s="2" t="n">
         <v>44370</v>
       </c>
-      <c r="C261" t="n">
-        <v>1.186645890305361</v>
-      </c>
+      <c r="C261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -3311,9 +3299,7 @@
       <c r="B263" s="2" t="n">
         <v>44372</v>
       </c>
-      <c r="C263" t="n">
-        <v>1.187784518615768</v>
-      </c>
+      <c r="C263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -3322,9 +3308,7 @@
       <c r="B264" s="2" t="n">
         <v>44376</v>
       </c>
-      <c r="C264" t="n">
-        <v>1.186896013045647</v>
-      </c>
+      <c r="C264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -3333,9 +3317,7 @@
       <c r="B265" s="2" t="n">
         <v>44379</v>
       </c>
-      <c r="C265" t="n">
-        <v>1.184696257406701</v>
-      </c>
+      <c r="C265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -3345,7 +3327,7 @@
         <v>44382</v>
       </c>
       <c r="C266" t="n">
-        <v>1.186306141666193</v>
+        <v>1.45353544492599</v>
       </c>
     </row>
     <row r="267">
@@ -3355,9 +3337,7 @@
       <c r="B267" s="2" t="n">
         <v>44385</v>
       </c>
-      <c r="C267" t="n">
-        <v>1.188123271786056</v>
-      </c>
+      <c r="C267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -3366,9 +3346,7 @@
       <c r="B268" s="2" t="n">
         <v>44396</v>
       </c>
-      <c r="C268" t="n">
-        <v>1.196279316745725</v>
-      </c>
+      <c r="C268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -3378,7 +3356,7 @@
         <v>44399</v>
       </c>
       <c r="C269" t="n">
-        <v>1.193847543608601</v>
+        <v>1.445462585189754</v>
       </c>
     </row>
     <row r="270">
@@ -3389,7 +3367,7 @@
         <v>44405</v>
       </c>
       <c r="C270" t="n">
-        <v>1.175904037815823</v>
+        <v>1.390172339945918</v>
       </c>
     </row>
     <row r="271">
@@ -3400,7 +3378,7 @@
         <v>44407</v>
       </c>
       <c r="C271" t="n">
-        <v>1.171678850480441</v>
+        <v>1.350386366519255</v>
       </c>
     </row>
     <row r="272">
@@ -3411,7 +3389,7 @@
         <v>44410</v>
       </c>
       <c r="C272" t="n">
-        <v>1.169679751972631</v>
+        <v>1.337819137461779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed pylint logging-not-lazy messages [fix #5]
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_x_large_portfolio_complexity_data.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_x_large_portfolio_complexity_data.xlsx
@@ -1895,7 +1895,7 @@
         <v>43765</v>
       </c>
       <c r="C134" t="n">
-        <v>1.160146352695709</v>
+        <v>1.16015630359837</v>
       </c>
     </row>
     <row r="135">
@@ -2016,7 +2016,7 @@
         <v>43826</v>
       </c>
       <c r="C145" t="n">
-        <v>1.168885292845949</v>
+        <v>1.171881684295534</v>
       </c>
     </row>
     <row r="146">
@@ -2027,7 +2027,7 @@
         <v>43833</v>
       </c>
       <c r="C146" t="n">
-        <v>1.180284271793053</v>
+        <v>1.183223386140115</v>
       </c>
     </row>
     <row r="147">
@@ -2038,7 +2038,7 @@
         <v>43836</v>
       </c>
       <c r="C147" t="n">
-        <v>1.21486052238984</v>
+        <v>1.217823389384934</v>
       </c>
     </row>
     <row r="148">
@@ -2093,7 +2093,7 @@
         <v>43862</v>
       </c>
       <c r="C152" t="n">
-        <v>1.236062985667228</v>
+        <v>1.238565299552142</v>
       </c>
     </row>
     <row r="153">
@@ -2104,7 +2104,7 @@
         <v>43864</v>
       </c>
       <c r="C153" t="n">
-        <v>1.224510215525612</v>
+        <v>1.226948046732958</v>
       </c>
     </row>
     <row r="154">
@@ -2115,7 +2115,7 @@
         <v>43866</v>
       </c>
       <c r="C154" t="n">
-        <v>1.22415486547171</v>
+        <v>1.226648974683219</v>
       </c>
     </row>
     <row r="155">
@@ -2137,7 +2137,7 @@
         <v>43871</v>
       </c>
       <c r="C156" t="n">
-        <v>1.23730038985183</v>
+        <v>1.239783964768033</v>
       </c>
     </row>
     <row r="157">
@@ -2148,7 +2148,7 @@
         <v>43874</v>
       </c>
       <c r="C157" t="n">
-        <v>1.228944539426958</v>
+        <v>1.231341914339102</v>
       </c>
     </row>
     <row r="158">
@@ -2170,7 +2170,7 @@
         <v>43894</v>
       </c>
       <c r="C159" t="n">
-        <v>1.224516623136881</v>
+        <v>1.224596937211389</v>
       </c>
     </row>
     <row r="160">
@@ -2181,7 +2181,7 @@
         <v>43896</v>
       </c>
       <c r="C160" t="n">
-        <v>1.22466122937041</v>
+        <v>1.22466650227657</v>
       </c>
     </row>
     <row r="161">
@@ -2192,7 +2192,7 @@
         <v>43903</v>
       </c>
       <c r="C161" t="n">
-        <v>1.235914030567496</v>
+        <v>1.235755952803562</v>
       </c>
     </row>
     <row r="162">
@@ -2203,7 +2203,7 @@
         <v>43906</v>
       </c>
       <c r="C162" t="n">
-        <v>1.208582765258972</v>
+        <v>1.207394298574729</v>
       </c>
     </row>
     <row r="163">
@@ -2225,7 +2225,7 @@
         <v>43908</v>
       </c>
       <c r="C164" t="n">
-        <v>1.223339205264765</v>
+        <v>1.221464327955706</v>
       </c>
     </row>
     <row r="165">
@@ -2236,7 +2236,7 @@
         <v>43909</v>
       </c>
       <c r="C165" t="n">
-        <v>1.224129108051137</v>
+        <v>1.220614369390921</v>
       </c>
     </row>
     <row r="166">
@@ -2247,7 +2247,7 @@
         <v>43910</v>
       </c>
       <c r="C166" t="n">
-        <v>1.235573301768256</v>
+        <v>1.232256445635086</v>
       </c>
     </row>
     <row r="167">
@@ -2280,7 +2280,7 @@
         <v>43917</v>
       </c>
       <c r="C169" t="n">
-        <v>1.257528759579208</v>
+        <v>1.25329796961472</v>
       </c>
     </row>
     <row r="170">
@@ -2291,7 +2291,7 @@
         <v>43924</v>
       </c>
       <c r="C170" t="n">
-        <v>1.254173798833946</v>
+        <v>1.248173324851996</v>
       </c>
     </row>
     <row r="171">
@@ -2302,7 +2302,7 @@
         <v>43936</v>
       </c>
       <c r="C171" t="n">
-        <v>1.251508208390669</v>
+        <v>1.244793804339156</v>
       </c>
     </row>
     <row r="172">
@@ -2357,7 +2357,7 @@
         <v>43987</v>
       </c>
       <c r="C176" t="n">
-        <v>1.249623747082607</v>
+        <v>1.240701803075182</v>
       </c>
     </row>
     <row r="177">
@@ -2368,7 +2368,7 @@
         <v>43990</v>
       </c>
       <c r="C177" t="n">
-        <v>1.249577153948315</v>
+        <v>1.239882725373991</v>
       </c>
     </row>
     <row r="178">
@@ -2379,7 +2379,7 @@
         <v>43993</v>
       </c>
       <c r="C178" t="n">
-        <v>1.24948293342525</v>
+        <v>1.239229319877219</v>
       </c>
     </row>
     <row r="179">
@@ -2423,7 +2423,7 @@
         <v>44019</v>
       </c>
       <c r="C182" t="n">
-        <v>1.242066799159612</v>
+        <v>1.232453600326134</v>
       </c>
     </row>
     <row r="183">
@@ -2434,7 +2434,7 @@
         <v>44025</v>
       </c>
       <c r="C183" t="n">
-        <v>1.24183318653802</v>
+        <v>1.231111004911923</v>
       </c>
     </row>
     <row r="184">
@@ -2467,7 +2467,7 @@
         <v>44055</v>
       </c>
       <c r="C186" t="n">
-        <v>1.239565513799398</v>
+        <v>1.228182306305312</v>
       </c>
     </row>
     <row r="187">
@@ -2478,7 +2478,7 @@
         <v>44064</v>
       </c>
       <c r="C187" t="n">
-        <v>1.226372595977206</v>
+        <v>1.214760197372009</v>
       </c>
     </row>
     <row r="188">
@@ -2489,7 +2489,7 @@
         <v>44067</v>
       </c>
       <c r="C188" t="n">
-        <v>1.22690209228363</v>
+        <v>1.214737649731441</v>
       </c>
     </row>
     <row r="189">
@@ -2500,7 +2500,7 @@
         <v>44085</v>
       </c>
       <c r="C189" t="n">
-        <v>1.22779570041693</v>
+        <v>1.216393863917958</v>
       </c>
     </row>
     <row r="190">
@@ -2533,7 +2533,7 @@
         <v>44097</v>
       </c>
       <c r="C192" t="n">
-        <v>1.227545350993828</v>
+        <v>1.215058924347624</v>
       </c>
     </row>
     <row r="193">
@@ -2566,7 +2566,7 @@
         <v>44145</v>
       </c>
       <c r="C195" t="n">
-        <v>1.202035027553715</v>
+        <v>1.192994489511771</v>
       </c>
     </row>
     <row r="196">
@@ -2588,7 +2588,7 @@
         <v>44149</v>
       </c>
       <c r="C197" t="n">
-        <v>1.192073467763204</v>
+        <v>1.200778399893643</v>
       </c>
     </row>
     <row r="198">
@@ -2599,7 +2599,7 @@
         <v>44155</v>
       </c>
       <c r="C198" t="n">
-        <v>1.193851112784309</v>
+        <v>1.201298852090896</v>
       </c>
     </row>
     <row r="199">
@@ -2610,7 +2610,7 @@
         <v>44158</v>
       </c>
       <c r="C199" t="n">
-        <v>1.182983355163583</v>
+        <v>1.189944379082265</v>
       </c>
     </row>
     <row r="200">
@@ -2621,7 +2621,7 @@
         <v>44159</v>
       </c>
       <c r="C200" t="n">
-        <v>1.182850136424509</v>
+        <v>1.189737156749509</v>
       </c>
     </row>
     <row r="201">
@@ -2654,7 +2654,7 @@
         <v>44162</v>
       </c>
       <c r="C203" t="n">
-        <v>1.155293426993963</v>
+        <v>1.172792111377981</v>
       </c>
     </row>
     <row r="204">
@@ -2665,7 +2665,7 @@
         <v>44181</v>
       </c>
       <c r="C204" t="n">
-        <v>1.158447683640106</v>
+        <v>1.172445011799087</v>
       </c>
     </row>
     <row r="205">
@@ -2676,7 +2676,7 @@
         <v>44182</v>
       </c>
       <c r="C205" t="n">
-        <v>1.158721805390498</v>
+        <v>1.172236581417402</v>
       </c>
     </row>
     <row r="206">
@@ -2687,7 +2687,7 @@
         <v>44186</v>
       </c>
       <c r="C206" t="n">
-        <v>1.160352133350743</v>
+        <v>1.173352039679966</v>
       </c>
     </row>
     <row r="207">
@@ -2808,7 +2808,7 @@
         <v>44252</v>
       </c>
       <c r="C217" t="n">
-        <v>1.263445535777546</v>
+        <v>1.246098319938603</v>
       </c>
     </row>
     <row r="218">
@@ -2940,7 +2940,7 @@
         <v>44298</v>
       </c>
       <c r="C229" t="n">
-        <v>1.210319165117816</v>
+        <v>1.234106195769172</v>
       </c>
     </row>
     <row r="230">
@@ -2951,7 +2951,7 @@
         <v>44301</v>
       </c>
       <c r="C230" t="n">
-        <v>1.220889966517364</v>
+        <v>1.243915096776673</v>
       </c>
     </row>
     <row r="231">
@@ -2962,7 +2962,7 @@
         <v>44302</v>
       </c>
       <c r="C231" t="n">
-        <v>1.209350538239505</v>
+        <v>1.232196760535111</v>
       </c>
     </row>
     <row r="232">
@@ -2973,7 +2973,7 @@
         <v>44305</v>
       </c>
       <c r="C232" t="n">
-        <v>1.208327948655497</v>
+        <v>1.231773395209215</v>
       </c>
     </row>
     <row r="233">
@@ -2984,7 +2984,7 @@
         <v>44308</v>
       </c>
       <c r="C233" t="n">
-        <v>1.207513369285311</v>
+        <v>1.230970572546587</v>
       </c>
     </row>
     <row r="234">
@@ -2995,7 +2995,7 @@
         <v>44313</v>
       </c>
       <c r="C234" t="n">
-        <v>1.254963718808026</v>
+        <v>1.279618645617331</v>
       </c>
     </row>
     <row r="235">
@@ -3006,7 +3006,7 @@
         <v>44316</v>
       </c>
       <c r="C235" t="n">
-        <v>1.2541140304283</v>
+        <v>1.2784050279892</v>
       </c>
     </row>
     <row r="236">
@@ -3017,7 +3017,7 @@
         <v>44319</v>
       </c>
       <c r="C236" t="n">
-        <v>1.252689620250149</v>
+        <v>1.277137095063419</v>
       </c>
     </row>
     <row r="237">
@@ -3028,7 +3028,7 @@
         <v>44320</v>
       </c>
       <c r="C237" t="n">
-        <v>1.251961778778859</v>
+        <v>1.276944327719232</v>
       </c>
     </row>
     <row r="238">
@@ -3039,7 +3039,7 @@
         <v>44321</v>
       </c>
       <c r="C238" t="n">
-        <v>1.251876098844296</v>
+        <v>1.276376505831042</v>
       </c>
     </row>
     <row r="239">
@@ -3094,7 +3094,7 @@
         <v>44333</v>
       </c>
       <c r="C243" t="n">
-        <v>1.299960470038234</v>
+        <v>1.324234935714067</v>
       </c>
     </row>
     <row r="244">
@@ -3105,7 +3105,7 @@
         <v>44334</v>
       </c>
       <c r="C244" t="n">
-        <v>1.337909672269377</v>
+        <v>1.362440657575851</v>
       </c>
     </row>
     <row r="245">
@@ -3116,7 +3116,7 @@
         <v>44335</v>
       </c>
       <c r="C245" t="n">
-        <v>1.350402306315797</v>
+        <v>1.374679267038917</v>
       </c>
     </row>
     <row r="246">
@@ -3127,7 +3127,7 @@
         <v>44336</v>
       </c>
       <c r="C246" t="n">
-        <v>1.374317018280406</v>
+        <v>1.399645712324217</v>
       </c>
     </row>
     <row r="247">
@@ -3138,7 +3138,7 @@
         <v>44337</v>
       </c>
       <c r="C247" t="n">
-        <v>1.37166063009448</v>
+        <v>1.397681023133019</v>
       </c>
     </row>
     <row r="248">
@@ -3149,7 +3149,7 @@
         <v>44340</v>
       </c>
       <c r="C248" t="n">
-        <v>1.396536135417827</v>
+        <v>1.423092640007945</v>
       </c>
     </row>
     <row r="249">
@@ -3160,7 +3160,7 @@
         <v>44341</v>
       </c>
       <c r="C249" t="n">
-        <v>1.406209022047955</v>
+        <v>1.434026161181842</v>
       </c>
     </row>
     <row r="250">
@@ -3171,7 +3171,7 @@
         <v>44343</v>
       </c>
       <c r="C250" t="n">
-        <v>1.404521719344106</v>
+        <v>1.432606268035194</v>
       </c>
     </row>
     <row r="251">
@@ -3182,7 +3182,7 @@
         <v>44347</v>
       </c>
       <c r="C251" t="n">
-        <v>1.488161909805113</v>
+        <v>1.519112145100228</v>
       </c>
     </row>
     <row r="252">
@@ -3237,7 +3237,7 @@
         <v>44357</v>
       </c>
       <c r="C256" t="n">
-        <v>1.521293420386913</v>
+        <v>1.488512669176378</v>
       </c>
     </row>
     <row r="257">
@@ -3270,7 +3270,7 @@
         <v>44365</v>
       </c>
       <c r="C259" t="n">
-        <v>1.565272833530306</v>
+        <v>1.528557167718977</v>
       </c>
     </row>
     <row r="260">

</xml_diff>

<commit_message>
added gprof2dot visualisation of profiling data
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_x_large_portfolio_complexity_data.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_x_large_portfolio_complexity_data.xlsx
@@ -2016,7 +2016,7 @@
         <v>43826</v>
       </c>
       <c r="C145" t="n">
-        <v>1.168885292845949</v>
+        <v>1.171881684295534</v>
       </c>
     </row>
     <row r="146">
@@ -2038,7 +2038,7 @@
         <v>43836</v>
       </c>
       <c r="C147" t="n">
-        <v>1.21486052238984</v>
+        <v>1.217823389384934</v>
       </c>
     </row>
     <row r="148">
@@ -2060,7 +2060,7 @@
         <v>43844</v>
       </c>
       <c r="C149" t="n">
-        <v>1.225847009048619</v>
+        <v>1.228879192361553</v>
       </c>
     </row>
     <row r="150">
@@ -2071,7 +2071,7 @@
         <v>43851</v>
       </c>
       <c r="C150" t="n">
-        <v>1.223997632247695</v>
+        <v>1.226892353205352</v>
       </c>
     </row>
     <row r="151">
@@ -2082,7 +2082,7 @@
         <v>43858</v>
       </c>
       <c r="C151" t="n">
-        <v>1.246643935962412</v>
+        <v>1.249117742245347</v>
       </c>
     </row>
     <row r="152">
@@ -2093,7 +2093,7 @@
         <v>43862</v>
       </c>
       <c r="C152" t="n">
-        <v>1.236072833604953</v>
+        <v>1.23607283366597</v>
       </c>
     </row>
     <row r="153">
@@ -2104,7 +2104,7 @@
         <v>43864</v>
       </c>
       <c r="C153" t="n">
-        <v>1.226948046732958</v>
+        <v>1.224510215525612</v>
       </c>
     </row>
     <row r="154">
@@ -2137,7 +2137,7 @@
         <v>43871</v>
       </c>
       <c r="C156" t="n">
-        <v>1.239783964768033</v>
+        <v>1.23730038985183</v>
       </c>
     </row>
     <row r="157">
@@ -2148,7 +2148,7 @@
         <v>43874</v>
       </c>
       <c r="C157" t="n">
-        <v>1.231341914339102</v>
+        <v>1.228944539426958</v>
       </c>
     </row>
     <row r="158">
@@ -2159,7 +2159,7 @@
         <v>43878</v>
       </c>
       <c r="C158" t="n">
-        <v>1.228113977519594</v>
+        <v>1.227174753504499</v>
       </c>
     </row>
     <row r="159">
@@ -2181,7 +2181,7 @@
         <v>43896</v>
       </c>
       <c r="C160" t="n">
-        <v>1.22466650227657</v>
+        <v>1.22466122937041</v>
       </c>
     </row>
     <row r="161">
@@ -2214,7 +2214,7 @@
         <v>43907</v>
       </c>
       <c r="C163" t="n">
-        <v>1.229196282763044</v>
+        <v>1.230561082727156</v>
       </c>
     </row>
     <row r="164">
@@ -2258,7 +2258,7 @@
         <v>43915</v>
       </c>
       <c r="C167" t="n">
-        <v>1.254837787206313</v>
+        <v>1.259691051498418</v>
       </c>
     </row>
     <row r="168">
@@ -2346,7 +2346,7 @@
         <v>43984</v>
       </c>
       <c r="C175" t="n">
-        <v>1.261125837412918</v>
+        <v>1.251640714470686</v>
       </c>
     </row>
     <row r="176">
@@ -2357,7 +2357,7 @@
         <v>43987</v>
       </c>
       <c r="C176" t="n">
-        <v>1.249623747082607</v>
+        <v>1.240701803075182</v>
       </c>
     </row>
     <row r="177">
@@ -2379,7 +2379,7 @@
         <v>43993</v>
       </c>
       <c r="C178" t="n">
-        <v>1.24948293342525</v>
+        <v>1.239229319877219</v>
       </c>
     </row>
     <row r="179">
@@ -2390,7 +2390,7 @@
         <v>43994</v>
       </c>
       <c r="C179" t="n">
-        <v>1.24989081645374</v>
+        <v>1.239385813920769</v>
       </c>
     </row>
     <row r="180">
@@ -2445,7 +2445,7 @@
         <v>44036</v>
       </c>
       <c r="C184" t="n">
-        <v>1.241279612420844</v>
+        <v>1.230371637033066</v>
       </c>
     </row>
     <row r="185">
@@ -2456,7 +2456,7 @@
         <v>44039</v>
       </c>
       <c r="C185" t="n">
-        <v>1.240343896002161</v>
+        <v>1.229065773288799</v>
       </c>
     </row>
     <row r="186">
@@ -2467,7 +2467,7 @@
         <v>44055</v>
       </c>
       <c r="C186" t="n">
-        <v>1.239565513799398</v>
+        <v>1.228182306305312</v>
       </c>
     </row>
     <row r="187">
@@ -2478,7 +2478,7 @@
         <v>44064</v>
       </c>
       <c r="C187" t="n">
-        <v>1.226372595977206</v>
+        <v>1.214760197372009</v>
       </c>
     </row>
     <row r="188">
@@ -2489,7 +2489,7 @@
         <v>44067</v>
       </c>
       <c r="C188" t="n">
-        <v>1.22690209228363</v>
+        <v>1.214737649731441</v>
       </c>
     </row>
     <row r="189">
@@ -2500,7 +2500,7 @@
         <v>44085</v>
       </c>
       <c r="C189" t="n">
-        <v>1.22779570041693</v>
+        <v>1.216393863917958</v>
       </c>
     </row>
     <row r="190">
@@ -2511,7 +2511,7 @@
         <v>44088</v>
       </c>
       <c r="C190" t="n">
-        <v>1.205641576628107</v>
+        <v>1.195224373986969</v>
       </c>
     </row>
     <row r="191">
@@ -2522,7 +2522,7 @@
         <v>44095</v>
       </c>
       <c r="C191" t="n">
-        <v>1.216840934226896</v>
+        <v>1.206114938435964</v>
       </c>
     </row>
     <row r="192">
@@ -2533,7 +2533,7 @@
         <v>44097</v>
       </c>
       <c r="C192" t="n">
-        <v>1.227545350993828</v>
+        <v>1.215058924347624</v>
       </c>
     </row>
     <row r="193">
@@ -2544,7 +2544,7 @@
         <v>44098</v>
       </c>
       <c r="C193" t="n">
-        <v>1.226995105162298</v>
+        <v>1.213940947482899</v>
       </c>
     </row>
     <row r="194">
@@ -2555,7 +2555,7 @@
         <v>44119</v>
       </c>
       <c r="C194" t="n">
-        <v>1.228583304476012</v>
+        <v>1.21513958041862</v>
       </c>
     </row>
     <row r="195">
@@ -2566,7 +2566,7 @@
         <v>44145</v>
       </c>
       <c r="C195" t="n">
-        <v>1.202035027553715</v>
+        <v>1.192994489511771</v>
       </c>
     </row>
     <row r="196">
@@ -2577,7 +2577,7 @@
         <v>44146</v>
       </c>
       <c r="C196" t="n">
-        <v>1.201453220846558</v>
+        <v>1.192555829941442</v>
       </c>
     </row>
     <row r="197">
@@ -2588,7 +2588,7 @@
         <v>44149</v>
       </c>
       <c r="C197" t="n">
-        <v>1.200773896767373</v>
+        <v>1.192073467763204</v>
       </c>
     </row>
     <row r="198">

</xml_diff>

<commit_message>
Reworked single date closing_price to fetch from prefetched_data or server_data
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_x_large_portfolio_complexity_data.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_x_large_portfolio_complexity_data.xlsx
@@ -1895,7 +1895,7 @@
         <v>43765</v>
       </c>
       <c r="C134" t="n">
-        <v>1.16015630359837</v>
+        <v>1.160150658571203</v>
       </c>
     </row>
     <row r="135">
@@ -2016,7 +2016,7 @@
         <v>43826</v>
       </c>
       <c r="C145" t="n">
-        <v>1.171881684295534</v>
+        <v>1.168885292845949</v>
       </c>
     </row>
     <row r="146">
@@ -2027,7 +2027,7 @@
         <v>43833</v>
       </c>
       <c r="C146" t="n">
-        <v>1.183223386140115</v>
+        <v>1.180284271793053</v>
       </c>
     </row>
     <row r="147">
@@ -2038,7 +2038,7 @@
         <v>43836</v>
       </c>
       <c r="C147" t="n">
-        <v>1.217823389384934</v>
+        <v>1.21486052238984</v>
       </c>
     </row>
     <row r="148">
@@ -2049,7 +2049,7 @@
         <v>43840</v>
       </c>
       <c r="C148" t="n">
-        <v>1.279036382914401</v>
+        <v>1.276010857199003</v>
       </c>
     </row>
     <row r="149">
@@ -2060,7 +2060,7 @@
         <v>43844</v>
       </c>
       <c r="C149" t="n">
-        <v>1.228879192361553</v>
+        <v>1.225847009048619</v>
       </c>
     </row>
     <row r="150">
@@ -2071,7 +2071,7 @@
         <v>43851</v>
       </c>
       <c r="C150" t="n">
-        <v>1.226892353205352</v>
+        <v>1.223997632247695</v>
       </c>
     </row>
     <row r="151">
@@ -2082,7 +2082,7 @@
         <v>43858</v>
       </c>
       <c r="C151" t="n">
-        <v>1.249117742245347</v>
+        <v>1.246643935962412</v>
       </c>
     </row>
     <row r="152">
@@ -2093,7 +2093,7 @@
         <v>43862</v>
       </c>
       <c r="C152" t="n">
-        <v>1.23607283366597</v>
+        <v>1.236062985667228</v>
       </c>
     </row>
     <row r="153">
@@ -2269,7 +2269,7 @@
         <v>43916</v>
       </c>
       <c r="C168" t="n">
-        <v>1.255368858611194</v>
+        <v>1.259233531562834</v>
       </c>
     </row>
     <row r="169">
@@ -2280,7 +2280,7 @@
         <v>43917</v>
       </c>
       <c r="C169" t="n">
-        <v>1.25329796961472</v>
+        <v>1.257528759579208</v>
       </c>
     </row>
     <row r="170">
@@ -2291,7 +2291,7 @@
         <v>43924</v>
       </c>
       <c r="C170" t="n">
-        <v>1.248173324851996</v>
+        <v>1.254173798833946</v>
       </c>
     </row>
     <row r="171">
@@ -2302,7 +2302,7 @@
         <v>43936</v>
       </c>
       <c r="C171" t="n">
-        <v>1.244793804339156</v>
+        <v>1.251508208390669</v>
       </c>
     </row>
     <row r="172">
@@ -2313,7 +2313,7 @@
         <v>43942</v>
       </c>
       <c r="C172" t="n">
-        <v>1.241089114964323</v>
+        <v>1.250056914663057</v>
       </c>
     </row>
     <row r="173">
@@ -2324,7 +2324,7 @@
         <v>43944</v>
       </c>
       <c r="C173" t="n">
-        <v>1.252630871270916</v>
+        <v>1.26130329888185</v>
       </c>
     </row>
     <row r="174">
@@ -2335,7 +2335,7 @@
         <v>43978</v>
       </c>
       <c r="C174" t="n">
-        <v>1.261138244488851</v>
+        <v>1.272806961088436</v>
       </c>
     </row>
     <row r="175">
@@ -2346,7 +2346,7 @@
         <v>43984</v>
       </c>
       <c r="C175" t="n">
-        <v>1.251640714470686</v>
+        <v>1.261125837412918</v>
       </c>
     </row>
     <row r="176">
@@ -2357,7 +2357,7 @@
         <v>43987</v>
       </c>
       <c r="C176" t="n">
-        <v>1.240701803075182</v>
+        <v>1.249623747082607</v>
       </c>
     </row>
     <row r="177">
@@ -2368,7 +2368,7 @@
         <v>43990</v>
       </c>
       <c r="C177" t="n">
-        <v>1.239882725373991</v>
+        <v>1.249577153948315</v>
       </c>
     </row>
     <row r="178">
@@ -2379,7 +2379,7 @@
         <v>43993</v>
       </c>
       <c r="C178" t="n">
-        <v>1.239229319877219</v>
+        <v>1.24948293342525</v>
       </c>
     </row>
     <row r="179">
@@ -2390,7 +2390,7 @@
         <v>43994</v>
       </c>
       <c r="C179" t="n">
-        <v>1.239385813920769</v>
+        <v>1.24989081645374</v>
       </c>
     </row>
     <row r="180">
@@ -2401,7 +2401,7 @@
         <v>44012</v>
       </c>
       <c r="C180" t="n">
-        <v>1.251827520035059</v>
+        <v>1.262322228572568</v>
       </c>
     </row>
     <row r="181">
@@ -2412,7 +2412,7 @@
         <v>44018</v>
       </c>
       <c r="C181" t="n">
-        <v>1.231903864561693</v>
+        <v>1.240854830291638</v>
       </c>
     </row>
     <row r="182">
@@ -2423,7 +2423,7 @@
         <v>44019</v>
       </c>
       <c r="C182" t="n">
-        <v>1.232453600326134</v>
+        <v>1.242066799159612</v>
       </c>
     </row>
     <row r="183">
@@ -2434,7 +2434,7 @@
         <v>44025</v>
       </c>
       <c r="C183" t="n">
-        <v>1.231111004911923</v>
+        <v>1.24183318653802</v>
       </c>
     </row>
     <row r="184">
@@ -2445,7 +2445,7 @@
         <v>44036</v>
       </c>
       <c r="C184" t="n">
-        <v>1.230371637033066</v>
+        <v>1.241279612420844</v>
       </c>
     </row>
     <row r="185">
@@ -2456,7 +2456,7 @@
         <v>44039</v>
       </c>
       <c r="C185" t="n">
-        <v>1.229065773288799</v>
+        <v>1.240343896002161</v>
       </c>
     </row>
     <row r="186">
@@ -2467,7 +2467,7 @@
         <v>44055</v>
       </c>
       <c r="C186" t="n">
-        <v>1.228182306305312</v>
+        <v>1.239565513799398</v>
       </c>
     </row>
     <row r="187">
@@ -2489,7 +2489,7 @@
         <v>44067</v>
       </c>
       <c r="C188" t="n">
-        <v>1.214737649731441</v>
+        <v>1.22690209228363</v>
       </c>
     </row>
     <row r="189">
@@ -2544,7 +2544,7 @@
         <v>44098</v>
       </c>
       <c r="C193" t="n">
-        <v>1.213940947482899</v>
+        <v>1.226995105162298</v>
       </c>
     </row>
     <row r="194">
@@ -2566,7 +2566,7 @@
         <v>44145</v>
       </c>
       <c r="C195" t="n">
-        <v>1.192994489511771</v>
+        <v>1.202035027553715</v>
       </c>
     </row>
     <row r="196">
@@ -2577,7 +2577,7 @@
         <v>44146</v>
       </c>
       <c r="C196" t="n">
-        <v>1.192555829941442</v>
+        <v>1.201453220846558</v>
       </c>
     </row>
     <row r="197">
@@ -2588,7 +2588,7 @@
         <v>44149</v>
       </c>
       <c r="C197" t="n">
-        <v>1.192073467763204</v>
+        <v>1.192073308631313</v>
       </c>
     </row>
     <row r="198">
@@ -2621,7 +2621,7 @@
         <v>44159</v>
       </c>
       <c r="C200" t="n">
-        <v>1.189737156749509</v>
+        <v>1.182850136424509</v>
       </c>
     </row>
     <row r="201">
@@ -2632,7 +2632,7 @@
         <v>44160</v>
       </c>
       <c r="C201" t="n">
-        <v>1.149225999358948</v>
+        <v>1.134412140823284</v>
       </c>
     </row>
     <row r="202">
@@ -2643,7 +2643,7 @@
         <v>44161</v>
       </c>
       <c r="C202" t="n">
-        <v>1.173906296295284</v>
+        <v>1.155892290501299</v>
       </c>
     </row>
     <row r="203">
@@ -2687,7 +2687,7 @@
         <v>44186</v>
       </c>
       <c r="C206" t="n">
-        <v>1.173352039679966</v>
+        <v>1.160352133350743</v>
       </c>
     </row>
     <row r="207">
@@ -2698,7 +2698,7 @@
         <v>44189</v>
       </c>
       <c r="C207" t="n">
-        <v>1.170979371306329</v>
+        <v>1.158309344632277</v>
       </c>
     </row>
     <row r="208">
@@ -2720,7 +2720,7 @@
         <v>44196</v>
       </c>
       <c r="C209" t="n">
-        <v>1.211399886366022</v>
+        <v>1.198220063701776</v>
       </c>
     </row>
     <row r="210">
@@ -2731,7 +2731,7 @@
         <v>44197</v>
       </c>
       <c r="C210" t="n">
-        <v>1.209062815901802</v>
+        <v>1.195588336915779</v>
       </c>
     </row>
     <row r="211">
@@ -2775,7 +2775,7 @@
         <v>44236</v>
       </c>
       <c r="C214" t="n">
-        <v>1.219685195887786</v>
+        <v>1.219626455980141</v>
       </c>
     </row>
     <row r="215">
@@ -2808,7 +2808,7 @@
         <v>44252</v>
       </c>
       <c r="C217" t="n">
-        <v>1.263445535777546</v>
+        <v>1.246098319938603</v>
       </c>
     </row>
     <row r="218">
@@ -2819,7 +2819,7 @@
         <v>44253</v>
       </c>
       <c r="C218" t="n">
-        <v>1.264352006479259</v>
+        <v>1.246273242820492</v>
       </c>
     </row>
     <row r="219">
@@ -2874,7 +2874,7 @@
         <v>44278</v>
       </c>
       <c r="C223" t="n">
-        <v>1.278942049283157</v>
+        <v>1.261691503158172</v>
       </c>
     </row>
     <row r="224">
@@ -2896,7 +2896,7 @@
         <v>44285</v>
       </c>
       <c r="C225" t="n">
-        <v>1.225329112322245</v>
+        <v>1.209662791130737</v>
       </c>
     </row>
     <row r="226">
@@ -2907,7 +2907,7 @@
         <v>44286</v>
       </c>
       <c r="C226" t="n">
-        <v>1.22508264222341</v>
+        <v>1.209156750441042</v>
       </c>
     </row>
     <row r="227">
@@ -2962,7 +2962,7 @@
         <v>44302</v>
       </c>
       <c r="C231" t="n">
-        <v>1.232196760535111</v>
+        <v>1.209350538239505</v>
       </c>
     </row>
     <row r="232">
@@ -2973,7 +2973,7 @@
         <v>44305</v>
       </c>
       <c r="C232" t="n">
-        <v>1.231773395209215</v>
+        <v>1.208327948655497</v>
       </c>
     </row>
     <row r="233">
@@ -2984,7 +2984,7 @@
         <v>44308</v>
       </c>
       <c r="C233" t="n">
-        <v>1.230970572546587</v>
+        <v>1.207513369285311</v>
       </c>
     </row>
     <row r="234">
@@ -3006,7 +3006,7 @@
         <v>44316</v>
       </c>
       <c r="C235" t="n">
-        <v>1.2784050279892</v>
+        <v>1.2541140304283</v>
       </c>
     </row>
     <row r="236">
@@ -3017,7 +3017,7 @@
         <v>44319</v>
       </c>
       <c r="C236" t="n">
-        <v>1.277137095063419</v>
+        <v>1.252689620250149</v>
       </c>
     </row>
     <row r="237">
@@ -3028,7 +3028,7 @@
         <v>44320</v>
       </c>
       <c r="C237" t="n">
-        <v>1.276944327719232</v>
+        <v>1.251961778778859</v>
       </c>
     </row>
     <row r="238">
@@ -3039,7 +3039,7 @@
         <v>44321</v>
       </c>
       <c r="C238" t="n">
-        <v>1.276376505831042</v>
+        <v>1.251876098844296</v>
       </c>
     </row>
     <row r="239">
@@ -3072,7 +3072,7 @@
         <v>44327</v>
       </c>
       <c r="C241" t="n">
-        <v>1.286615558881463</v>
+        <v>1.262663169287868</v>
       </c>
     </row>
     <row r="242">
@@ -3094,7 +3094,7 @@
         <v>44333</v>
       </c>
       <c r="C243" t="n">
-        <v>1.324234935714067</v>
+        <v>1.299960470038234</v>
       </c>
     </row>
     <row r="244">
@@ -3116,7 +3116,7 @@
         <v>44335</v>
       </c>
       <c r="C245" t="n">
-        <v>1.374679267038917</v>
+        <v>1.350402306315797</v>
       </c>
     </row>
     <row r="246">
@@ -3127,7 +3127,7 @@
         <v>44336</v>
       </c>
       <c r="C246" t="n">
-        <v>1.399645712324217</v>
+        <v>1.374317018280406</v>
       </c>
     </row>
     <row r="247">
@@ -3171,7 +3171,7 @@
         <v>44343</v>
       </c>
       <c r="C250" t="n">
-        <v>1.432606268035194</v>
+        <v>1.404521719344106</v>
       </c>
     </row>
     <row r="251">
@@ -3182,7 +3182,7 @@
         <v>44347</v>
       </c>
       <c r="C251" t="n">
-        <v>1.519112145100228</v>
+        <v>1.488161909805113</v>
       </c>
     </row>
     <row r="252">
@@ -3215,7 +3215,7 @@
         <v>44351</v>
       </c>
       <c r="C254" t="n">
-        <v>1.497422404599028</v>
+        <v>1.46652171772181</v>
       </c>
     </row>
     <row r="255">
@@ -3248,7 +3248,7 @@
         <v>44362</v>
       </c>
       <c r="C257" t="n">
-        <v>1.565272195641491</v>
+        <v>1.529561818741367</v>
       </c>
     </row>
     <row r="258">
@@ -3281,7 +3281,7 @@
         <v>44369</v>
       </c>
       <c r="C260" t="n">
-        <v>1.511848028050094</v>
+        <v>1.48817942768943</v>
       </c>
     </row>
     <row r="261">
@@ -3292,7 +3292,7 @@
         <v>44370</v>
       </c>
       <c r="C261" t="n">
-        <v>1.518667350800931</v>
+        <v>1.500564367995939</v>
       </c>
     </row>
     <row r="262">
@@ -3303,7 +3303,7 @@
         <v>44371</v>
       </c>
       <c r="C262" t="n">
-        <v>1.517943032579118</v>
+        <v>1.49977571503411</v>
       </c>
     </row>
     <row r="263">

</xml_diff>